<commit_message>
Agent Domain Extractor Scripts Created
</commit_message>
<xml_diff>
--- a/Parser/rule_baseV0.2.xlsx
+++ b/Parser/rule_baseV0.2.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27230"/>
   <workbookPr date1904="1" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ayushdas/Desktop/PPI_DB/Parser/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="620" yWindow="-18920" windowWidth="26740" windowHeight="14660" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Abundance" sheetId="1" r:id="rId1"/>
@@ -13,11 +18,14 @@
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
@@ -3697,12 +3705,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="#,##0"/>
-  </numFmts>
-  <fonts count="25">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -3863,49 +3867,54 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="22">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -4228,23 +4237,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="95" workbookViewId="0">
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="20.140625" customWidth="1"/>
-    <col min="2" max="3" width="10.140625" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" customWidth="1"/>
-    <col min="6" max="1025" width="10.140625" customWidth="1"/>
+    <col min="1" max="1" width="20.1640625" customWidth="1"/>
+    <col min="2" max="3" width="10.1640625" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" customWidth="1"/>
+    <col min="5" max="5" width="10.5" customWidth="1"/>
+    <col min="6" max="1025" width="10.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>1052</v>
       </c>
@@ -4261,7 +4270,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>1057</v>
       </c>
@@ -4272,7 +4281,7 @@
         <v>21258328</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>1059</v>
       </c>
@@ -4283,7 +4292,7 @@
         <v>21258328</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>1061</v>
       </c>
@@ -4294,7 +4303,7 @@
         <v>21258328</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>1063</v>
       </c>
@@ -4305,7 +4314,7 @@
         <v>14657186</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>1065</v>
       </c>
@@ -4316,7 +4325,7 @@
         <v>17243894</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>1067</v>
       </c>
@@ -4327,12 +4336,12 @@
         <v>17243894</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>1069</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>1070</v>
       </c>
@@ -4343,7 +4352,7 @@
         <v>17243894</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>1072</v>
       </c>
@@ -4354,7 +4363,7 @@
         <v>17243894</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>1074</v>
       </c>
@@ -4365,7 +4374,7 @@
         <v>17243894</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>1075</v>
       </c>
@@ -4376,7 +4385,7 @@
         <v>17243894</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>1076</v>
       </c>
@@ -4387,7 +4396,7 @@
         <v>17243894</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>1078</v>
       </c>
@@ -4398,7 +4407,7 @@
         <v>17243894</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>1080</v>
       </c>
@@ -4409,7 +4418,7 @@
         <v>17243894</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>1081</v>
       </c>
@@ -4420,7 +4429,7 @@
         <v>17243894</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>1082</v>
       </c>
@@ -4431,7 +4440,7 @@
         <v>17243894</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>1083</v>
       </c>
@@ -4442,7 +4451,7 @@
         <v>17243894</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>1085</v>
       </c>
@@ -4453,7 +4462,7 @@
         <v>17243894</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>1087</v>
       </c>
@@ -4464,7 +4473,7 @@
         <v>17243894</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>1089</v>
       </c>
@@ -4476,41 +4485,35 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="24" type="noConversion"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Normál"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normál"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="20.140625" customWidth="1"/>
-    <col min="2" max="2" width="37.140625" customWidth="1"/>
-    <col min="3" max="3" width="23.5703125" customWidth="1"/>
-    <col min="4" max="4" width="45.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1"/>
-    <col min="6" max="6" width="25.85546875" customWidth="1"/>
-    <col min="7" max="1025" width="10.5703125" customWidth="1"/>
+    <col min="1" max="1" width="20.1640625" customWidth="1"/>
+    <col min="2" max="2" width="37.1640625" customWidth="1"/>
+    <col min="3" max="3" width="23.5" customWidth="1"/>
+    <col min="4" max="4" width="45.5" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" customWidth="1"/>
+    <col min="6" max="6" width="25.83203125" customWidth="1"/>
+    <col min="7" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>1052</v>
       </c>
@@ -4536,7 +4539,7 @@
         <v>1096</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>1057</v>
       </c>
@@ -4556,7 +4559,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>1101</v>
       </c>
@@ -4582,7 +4585,7 @@
         <v>1105</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>1061</v>
       </c>
@@ -4605,7 +4608,7 @@
         <v>21258328</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>1109</v>
       </c>
@@ -4631,7 +4634,7 @@
         <v>1114</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>1115</v>
       </c>
@@ -4651,7 +4654,7 @@
         <v>1119</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>1120</v>
       </c>
@@ -4671,7 +4674,7 @@
         <v>1012</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>1013</v>
       </c>
@@ -4691,7 +4694,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>1065</v>
       </c>
@@ -4717,7 +4720,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>1067</v>
       </c>
@@ -4740,7 +4743,7 @@
         <v>17243894</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>1069</v>
       </c>
@@ -4760,7 +4763,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>1027</v>
       </c>
@@ -4783,7 +4786,7 @@
         <v>17243894</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>1072</v>
       </c>
@@ -4806,7 +4809,7 @@
         <v>17243894</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>1074</v>
       </c>
@@ -4829,7 +4832,7 @@
         <v>17243894</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>1075</v>
       </c>
@@ -4852,7 +4855,7 @@
         <v>17243894</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>1076</v>
       </c>
@@ -4875,7 +4878,7 @@
         <v>17243894</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>1043</v>
       </c>
@@ -4895,7 +4898,7 @@
         <v>1047</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>1048</v>
       </c>
@@ -4915,7 +4918,7 @@
         <v>1051</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>964</v>
       </c>
@@ -4935,7 +4938,7 @@
         <v>967</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>968</v>
       </c>
@@ -4955,7 +4958,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>973</v>
       </c>
@@ -4975,7 +4978,7 @@
         <v>977</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>978</v>
       </c>
@@ -4995,7 +4998,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>983</v>
       </c>
@@ -5015,7 +5018,7 @@
         <v>986</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>1078</v>
       </c>
@@ -5038,7 +5041,7 @@
         <v>17243894</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>1080</v>
       </c>
@@ -5061,7 +5064,7 @@
         <v>17243894</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>1081</v>
       </c>
@@ -5084,7 +5087,7 @@
         <v>17243894</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>1082</v>
       </c>
@@ -5107,7 +5110,7 @@
         <v>17243894</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>999</v>
       </c>
@@ -5127,7 +5130,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>1083</v>
       </c>
@@ -5150,7 +5153,7 @@
         <v>17243894</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>1085</v>
       </c>
@@ -5173,7 +5176,7 @@
         <v>17243894</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>923</v>
       </c>
@@ -5193,7 +5196,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>1087</v>
       </c>
@@ -5216,7 +5219,7 @@
         <v>17243894</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>931</v>
       </c>
@@ -5236,7 +5239,7 @@
         <v>935</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>936</v>
       </c>
@@ -5256,7 +5259,7 @@
         <v>940</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>941</v>
       </c>
@@ -5276,7 +5279,7 @@
         <v>944</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>945</v>
       </c>
@@ -5296,7 +5299,7 @@
         <v>948</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>949</v>
       </c>
@@ -5313,7 +5316,7 @@
         <v>951</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
         <v>952</v>
       </c>
@@ -5336,7 +5339,7 @@
         <v>17243894</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
         <v>1089</v>
       </c>
@@ -5356,7 +5359,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
         <v>957</v>
       </c>
@@ -5376,7 +5379,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>961</v>
       </c>
@@ -5396,7 +5399,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
         <v>865</v>
       </c>
@@ -5416,7 +5419,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
         <v>869</v>
       </c>
@@ -5436,7 +5439,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
         <v>874</v>
       </c>
@@ -5456,7 +5459,7 @@
         <v>877</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
         <v>878</v>
       </c>
@@ -5476,7 +5479,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
         <v>882</v>
       </c>
@@ -5496,7 +5499,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
         <v>886</v>
       </c>
@@ -5516,7 +5519,7 @@
         <v>889</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
         <v>890</v>
       </c>
@@ -5536,7 +5539,7 @@
         <v>893</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
         <v>894</v>
       </c>
@@ -5556,7 +5559,7 @@
         <v>897</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="16">
+    <row r="50" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>898</v>
       </c>
@@ -5576,7 +5579,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A51" t="s">
         <v>902</v>
       </c>
@@ -5596,7 +5599,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A52" t="s">
         <v>906</v>
       </c>
@@ -5616,7 +5619,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="15">
+    <row r="53" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>910</v>
       </c>
@@ -5636,7 +5639,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="16">
+    <row r="54" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>914</v>
       </c>
@@ -5656,7 +5659,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="16">
+    <row r="55" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>918</v>
       </c>
@@ -5676,7 +5679,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="16">
+    <row r="56" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>811</v>
       </c>
@@ -5696,7 +5699,7 @@
         <v>814</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="16">
+    <row r="57" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>815</v>
       </c>
@@ -5716,7 +5719,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="16">
+    <row r="58" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>819</v>
       </c>
@@ -5736,7 +5739,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="16">
+    <row r="59" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>823</v>
       </c>
@@ -5756,7 +5759,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="16">
+    <row r="60" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>827</v>
       </c>
@@ -5776,7 +5779,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="16">
+    <row r="61" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>832</v>
       </c>
@@ -5796,7 +5799,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="16">
+    <row r="62" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>836</v>
       </c>
@@ -5816,7 +5819,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="16">
+    <row r="63" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>841</v>
       </c>
@@ -5836,7 +5839,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="16">
+    <row r="64" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>845</v>
       </c>
@@ -5856,7 +5859,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="16">
+    <row r="65" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>849</v>
       </c>
@@ -5876,7 +5879,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="16">
+    <row r="66" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>853</v>
       </c>
@@ -5896,7 +5899,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="16">
+    <row r="67" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>858</v>
       </c>
@@ -5917,41 +5920,35 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="24" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M385"/>
   <sheetViews>
-    <sheetView topLeftCell="A133" workbookViewId="0">
-      <selection sqref="A1:H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1:N1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" customWidth="1"/>
-    <col min="5" max="5" width="34.85546875" customWidth="1"/>
-    <col min="6" max="6" width="75.140625" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" customWidth="1"/>
-    <col min="8" max="1025" width="10.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.5" customWidth="1"/>
+    <col min="2" max="2" width="18.5" customWidth="1"/>
+    <col min="3" max="3" width="15.5" customWidth="1"/>
+    <col min="4" max="4" width="10.5" customWidth="1"/>
+    <col min="5" max="5" width="34.83203125" customWidth="1"/>
+    <col min="6" max="6" width="75.1640625" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" customWidth="1"/>
+    <col min="8" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>862</v>
       </c>
@@ -5992,7 +5989,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>759</v>
       </c>
@@ -6024,7 +6021,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>766</v>
       </c>
@@ -6044,7 +6041,7 @@
         <v>21258328</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>770</v>
       </c>
@@ -6067,7 +6064,7 @@
         <v>21258328</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>774</v>
       </c>
@@ -6087,7 +6084,7 @@
         <v>21258328</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>777</v>
       </c>
@@ -6113,7 +6110,7 @@
         <v>21258328</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>782</v>
       </c>
@@ -6133,7 +6130,7 @@
         <v>21258328</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>785</v>
       </c>
@@ -6156,7 +6153,7 @@
         <v>21258328</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>789</v>
       </c>
@@ -6176,7 +6173,7 @@
         <v>21258328</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>792</v>
       </c>
@@ -6208,7 +6205,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>798</v>
       </c>
@@ -6228,7 +6225,7 @@
         <v>21258328</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>801</v>
       </c>
@@ -6248,7 +6245,7 @@
         <v>21258328</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>803</v>
       </c>
@@ -6268,7 +6265,7 @@
         <v>21258328</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>805</v>
       </c>
@@ -6288,7 +6285,7 @@
         <v>21258328</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>807</v>
       </c>
@@ -6308,7 +6305,7 @@
         <v>21258328</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>809</v>
       </c>
@@ -6328,7 +6325,7 @@
         <v>21258328</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>700</v>
       </c>
@@ -6348,7 +6345,7 @@
         <v>21258328</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="16">
+    <row r="26" spans="1:12" ht="18" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>702</v>
       </c>
@@ -6381,7 +6378,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>709</v>
       </c>
@@ -6404,7 +6401,7 @@
         <v>1317063</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>713</v>
       </c>
@@ -6421,7 +6418,7 @@
         <v>18769913</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>717</v>
       </c>
@@ -6435,7 +6432,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>721</v>
       </c>
@@ -6452,7 +6449,7 @@
         <v>18769913</v>
       </c>
     </row>
-    <row r="34" spans="1:13">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>725</v>
       </c>
@@ -6472,7 +6469,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="36" spans="1:13">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>730</v>
       </c>
@@ -6498,7 +6495,7 @@
         <v>1317063</v>
       </c>
     </row>
-    <row r="37" spans="1:13">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>735</v>
       </c>
@@ -6509,7 +6506,7 @@
         <v>1317063</v>
       </c>
     </row>
-    <row r="39" spans="1:13">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
         <v>737</v>
       </c>
@@ -6526,12 +6523,12 @@
         <v>740</v>
       </c>
     </row>
-    <row r="40" spans="1:13">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.15">
       <c r="L40" t="s">
         <v>741</v>
       </c>
     </row>
-    <row r="41" spans="1:13">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>742</v>
       </c>
@@ -6545,7 +6542,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="43" spans="1:13">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
         <v>746</v>
       </c>
@@ -6562,7 +6559,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="45" spans="1:13">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
         <v>658</v>
       </c>
@@ -6576,7 +6573,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="47" spans="1:13">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
         <v>662</v>
       </c>
@@ -6590,7 +6587,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="49" spans="1:12">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
         <v>666</v>
       </c>
@@ -6607,7 +6604,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="51" spans="1:12" ht="17">
+    <row r="51" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>670</v>
       </c>
@@ -6636,12 +6633,12 @@
         <v>676</v>
       </c>
     </row>
-    <row r="52" spans="1:12" ht="17">
+    <row r="52" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="H52" s="9" t="s">
         <v>677</v>
       </c>
     </row>
-    <row r="53" spans="1:12">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A53" t="s">
         <v>678</v>
       </c>
@@ -6655,7 +6652,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="55" spans="1:12">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A55" t="s">
         <v>682</v>
       </c>
@@ -6669,7 +6666,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="57" spans="1:12">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A57" t="s">
         <v>686</v>
       </c>
@@ -6683,7 +6680,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="59" spans="1:12" ht="15">
+    <row r="59" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>690</v>
       </c>
@@ -6709,7 +6706,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="60" spans="1:12" ht="21">
+    <row r="60" spans="1:12" ht="21" x14ac:dyDescent="0.25">
       <c r="F60" t="s">
         <v>696</v>
       </c>
@@ -6723,7 +6720,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="21">
+    <row r="61" spans="1:12" ht="21" x14ac:dyDescent="0.25">
       <c r="F61" t="s">
         <v>619</v>
       </c>
@@ -6737,7 +6734,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="63" spans="1:12">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A63" t="s">
         <v>622</v>
       </c>
@@ -6751,7 +6748,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="65" spans="1:6">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A65" t="s">
         <v>626</v>
       </c>
@@ -6765,7 +6762,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="67" spans="1:6">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A67" t="s">
         <v>630</v>
       </c>
@@ -6779,7 +6776,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="69" spans="1:6">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A69" t="s">
         <v>634</v>
       </c>
@@ -6793,7 +6790,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="71" spans="1:6">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A71" t="s">
         <v>638</v>
       </c>
@@ -6807,7 +6804,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="73" spans="1:6">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A73" t="s">
         <v>642</v>
       </c>
@@ -6821,7 +6818,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="75" spans="1:6">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A75" t="s">
         <v>646</v>
       </c>
@@ -6841,7 +6838,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="77" spans="1:6">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A77" t="s">
         <v>650</v>
       </c>
@@ -6858,7 +6855,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="79" spans="1:6">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A79" t="s">
         <v>654</v>
       </c>
@@ -6875,7 +6872,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="81" spans="1:6">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A81" t="s">
         <v>557</v>
       </c>
@@ -6892,7 +6889,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="83" spans="1:6">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A83" t="s">
         <v>561</v>
       </c>
@@ -6909,7 +6906,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="85" spans="1:6">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A85" t="s">
         <v>565</v>
       </c>
@@ -6926,7 +6923,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="87" spans="1:6">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A87" t="s">
         <v>569</v>
       </c>
@@ -6943,7 +6940,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="89" spans="1:6">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A89" t="s">
         <v>573</v>
       </c>
@@ -6960,7 +6957,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="91" spans="1:6">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A91" t="s">
         <v>577</v>
       </c>
@@ -6977,7 +6974,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="93" spans="1:6">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A93" t="s">
         <v>581</v>
       </c>
@@ -6997,7 +6994,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="95" spans="1:6">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A95" t="s">
         <v>585</v>
       </c>
@@ -7011,7 +7008,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="97" spans="1:6">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A97" t="s">
         <v>589</v>
       </c>
@@ -7028,7 +7025,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="99" spans="1:6">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A99" t="s">
         <v>593</v>
       </c>
@@ -7045,7 +7042,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="101" spans="1:6">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A101" t="s">
         <v>597</v>
       </c>
@@ -7062,7 +7059,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="103" spans="1:6">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A103" t="s">
         <v>601</v>
       </c>
@@ -7079,7 +7076,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="105" spans="1:6">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A105" t="s">
         <v>605</v>
       </c>
@@ -7096,7 +7093,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="107" spans="1:6">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A107" t="s">
         <v>609</v>
       </c>
@@ -7116,7 +7113,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="109" spans="1:6">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A109" t="s">
         <v>613</v>
       </c>
@@ -7130,7 +7127,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="111" spans="1:6">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A111" t="s">
         <v>617</v>
       </c>
@@ -7147,7 +7144,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="113" spans="1:6">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A113" t="s">
         <v>491</v>
       </c>
@@ -7164,7 +7161,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="115" spans="1:6">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A115" t="s">
         <v>495</v>
       </c>
@@ -7181,7 +7178,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="117" spans="1:6">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A117" t="s">
         <v>499</v>
       </c>
@@ -7195,7 +7192,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="119" spans="1:6">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A119" t="s">
         <v>503</v>
       </c>
@@ -7212,7 +7209,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="121" spans="1:6">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A121" t="s">
         <v>507</v>
       </c>
@@ -7226,7 +7223,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="123" spans="1:6">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A123" t="s">
         <v>511</v>
       </c>
@@ -7240,7 +7237,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="125" spans="1:6">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A125" t="s">
         <v>515</v>
       </c>
@@ -7254,7 +7251,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="127" spans="1:6">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A127" t="s">
         <v>519</v>
       </c>
@@ -7271,7 +7268,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="129" spans="1:6">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A129" t="s">
         <v>522</v>
       </c>
@@ -7285,7 +7282,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="131" spans="1:6">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A131" t="s">
         <v>526</v>
       </c>
@@ -7302,7 +7299,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="133" spans="1:6">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A133" t="s">
         <v>530</v>
       </c>
@@ -7319,7 +7316,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="135" spans="1:6">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A135" t="s">
         <v>534</v>
       </c>
@@ -7333,7 +7330,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="137" spans="1:6">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A137" t="s">
         <v>538</v>
       </c>
@@ -7347,7 +7344,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="139" spans="1:6">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A139" t="s">
         <v>542</v>
       </c>
@@ -7364,7 +7361,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="141" spans="1:6">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A141" t="s">
         <v>546</v>
       </c>
@@ -7378,7 +7375,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="143" spans="1:6">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A143" t="s">
         <v>550</v>
       </c>
@@ -7395,7 +7392,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="145" spans="1:6">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A145" t="s">
         <v>554</v>
       </c>
@@ -7409,7 +7406,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="147" spans="1:6">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A147" t="s">
         <v>427</v>
       </c>
@@ -7423,7 +7420,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="149" spans="1:6">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A149" t="s">
         <v>431</v>
       </c>
@@ -7437,7 +7434,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="151" spans="1:6">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A151" t="s">
         <v>435</v>
       </c>
@@ -7454,7 +7451,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="153" spans="1:6">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A153" t="s">
         <v>440</v>
       </c>
@@ -7471,7 +7468,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="155" spans="1:6">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A155" t="s">
         <v>444</v>
       </c>
@@ -7488,7 +7485,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="157" spans="1:6">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A157" t="s">
         <v>448</v>
       </c>
@@ -7502,7 +7499,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="159" spans="1:6">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A159" t="s">
         <v>452</v>
       </c>
@@ -7516,7 +7513,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="161" spans="1:6">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A161" t="s">
         <v>456</v>
       </c>
@@ -7530,7 +7527,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="163" spans="1:6">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A163" t="s">
         <v>460</v>
       </c>
@@ -7544,7 +7541,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="165" spans="1:6">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A165" t="s">
         <v>464</v>
       </c>
@@ -7558,7 +7555,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="167" spans="1:6">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A167" t="s">
         <v>468</v>
       </c>
@@ -7575,7 +7572,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="169" spans="1:6">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A169" t="s">
         <v>471</v>
       </c>
@@ -7589,7 +7586,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="171" spans="1:6">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A171" t="s">
         <v>474</v>
       </c>
@@ -7606,7 +7603,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="173" spans="1:6">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A173" t="s">
         <v>478</v>
       </c>
@@ -7620,7 +7617,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="175" spans="1:6">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A175" t="s">
         <v>482</v>
       </c>
@@ -7634,7 +7631,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="177" spans="1:6">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A177" t="s">
         <v>486</v>
       </c>
@@ -7648,7 +7645,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="179" spans="1:6">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A179" t="s">
         <v>363</v>
       </c>
@@ -7662,7 +7659,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="181" spans="1:6">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A181" t="s">
         <v>367</v>
       </c>
@@ -7679,7 +7676,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="183" spans="1:6">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A183" t="s">
         <v>371</v>
       </c>
@@ -7696,7 +7693,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="185" spans="1:6">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A185" t="s">
         <v>375</v>
       </c>
@@ -7713,7 +7710,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="187" spans="1:6">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A187" t="s">
         <v>379</v>
       </c>
@@ -7730,7 +7727,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="189" spans="1:6">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A189" t="s">
         <v>383</v>
       </c>
@@ -7744,7 +7741,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="191" spans="1:6">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A191" t="s">
         <v>387</v>
       </c>
@@ -7761,7 +7758,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="193" spans="1:6">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A193" t="s">
         <v>391</v>
       </c>
@@ -7778,7 +7775,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="195" spans="1:6">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A195" t="s">
         <v>395</v>
       </c>
@@ -7795,7 +7792,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="197" spans="1:6">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A197" t="s">
         <v>399</v>
       </c>
@@ -7809,7 +7806,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="199" spans="1:6">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A199" t="s">
         <v>403</v>
       </c>
@@ -7823,7 +7820,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="201" spans="1:6">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A201" t="s">
         <v>407</v>
       </c>
@@ -7837,7 +7834,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="203" spans="1:6">
+    <row r="203" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A203" t="s">
         <v>411</v>
       </c>
@@ -7851,7 +7848,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="205" spans="1:6">
+    <row r="205" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A205" t="s">
         <v>415</v>
       </c>
@@ -7865,7 +7862,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="207" spans="1:6">
+    <row r="207" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A207" t="s">
         <v>419</v>
       </c>
@@ -7879,7 +7876,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="209" spans="1:6">
+    <row r="209" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A209" t="s">
         <v>423</v>
       </c>
@@ -7893,7 +7890,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="211" spans="1:6">
+    <row r="211" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A211" t="s">
         <v>300</v>
       </c>
@@ -7907,7 +7904,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="213" spans="1:6">
+    <row r="213" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A213" t="s">
         <v>304</v>
       </c>
@@ -7921,7 +7918,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="215" spans="1:6">
+    <row r="215" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A215" t="s">
         <v>308</v>
       </c>
@@ -7935,7 +7932,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="217" spans="1:6">
+    <row r="217" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A217" t="s">
         <v>312</v>
       </c>
@@ -7949,7 +7946,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="219" spans="1:6">
+    <row r="219" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A219" t="s">
         <v>316</v>
       </c>
@@ -7963,7 +7960,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="221" spans="1:6">
+    <row r="221" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A221" t="s">
         <v>320</v>
       </c>
@@ -7980,7 +7977,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="223" spans="1:6">
+    <row r="223" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A223" t="s">
         <v>324</v>
       </c>
@@ -7997,7 +7994,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="225" spans="1:6">
+    <row r="225" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A225" t="s">
         <v>328</v>
       </c>
@@ -8014,7 +8011,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="227" spans="1:6">
+    <row r="227" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A227" t="s">
         <v>332</v>
       </c>
@@ -8031,7 +8028,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="229" spans="1:6">
+    <row r="229" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A229" t="s">
         <v>336</v>
       </c>
@@ -8048,7 +8045,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="231" spans="1:6">
+    <row r="231" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A231" t="s">
         <v>340</v>
       </c>
@@ -8065,7 +8062,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="233" spans="1:6">
+    <row r="233" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A233" t="s">
         <v>344</v>
       </c>
@@ -8079,7 +8076,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="235" spans="1:6">
+    <row r="235" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A235" t="s">
         <v>348</v>
       </c>
@@ -8093,7 +8090,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="237" spans="1:6">
+    <row r="237" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A237" t="s">
         <v>352</v>
       </c>
@@ -8110,7 +8107,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="239" spans="1:6">
+    <row r="239" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A239" t="s">
         <v>356</v>
       </c>
@@ -8124,7 +8121,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="241" spans="1:6">
+    <row r="241" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A241" t="s">
         <v>360</v>
       </c>
@@ -8138,7 +8135,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="243" spans="1:6">
+    <row r="243" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A243" t="s">
         <v>237</v>
       </c>
@@ -8152,7 +8149,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="245" spans="1:6">
+    <row r="245" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A245" t="s">
         <v>241</v>
       </c>
@@ -8169,7 +8166,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="247" spans="1:6">
+    <row r="247" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A247" t="s">
         <v>245</v>
       </c>
@@ -8183,7 +8180,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="249" spans="1:6">
+    <row r="249" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A249" t="s">
         <v>249</v>
       </c>
@@ -8197,7 +8194,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="251" spans="1:6">
+    <row r="251" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A251" t="s">
         <v>253</v>
       </c>
@@ -8211,7 +8208,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="253" spans="1:6">
+    <row r="253" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A253" t="s">
         <v>257</v>
       </c>
@@ -8228,7 +8225,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="255" spans="1:6">
+    <row r="255" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A255" t="s">
         <v>261</v>
       </c>
@@ -8242,7 +8239,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="257" spans="1:6">
+    <row r="257" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A257" t="s">
         <v>265</v>
       </c>
@@ -8256,7 +8253,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="259" spans="1:6">
+    <row r="259" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A259" t="s">
         <v>269</v>
       </c>
@@ -8273,7 +8270,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="261" spans="1:6">
+    <row r="261" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A261" t="s">
         <v>274</v>
       </c>
@@ -8290,7 +8287,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="263" spans="1:6">
+    <row r="263" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A263" t="s">
         <v>278</v>
       </c>
@@ -8307,7 +8304,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="265" spans="1:6">
+    <row r="265" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A265" t="s">
         <v>281</v>
       </c>
@@ -8321,7 +8318,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="267" spans="1:6">
+    <row r="267" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A267" t="s">
         <v>285</v>
       </c>
@@ -8338,7 +8335,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="269" spans="1:6">
+    <row r="269" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A269" t="s">
         <v>289</v>
       </c>
@@ -8353,7 +8350,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="271" spans="1:6">
+    <row r="271" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A271" t="s">
         <v>293</v>
       </c>
@@ -8368,7 +8365,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="273" spans="1:7">
+    <row r="273" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A273" t="s">
         <v>297</v>
       </c>
@@ -8382,7 +8379,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="275" spans="1:7">
+    <row r="275" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A275" t="s">
         <v>174</v>
       </c>
@@ -8396,7 +8393,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="277" spans="1:7">
+    <row r="277" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A277" t="s">
         <v>178</v>
       </c>
@@ -8413,7 +8410,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="279" spans="1:7">
+    <row r="279" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A279" t="s">
         <v>182</v>
       </c>
@@ -8427,7 +8424,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="281" spans="1:7">
+    <row r="281" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A281" t="s">
         <v>186</v>
       </c>
@@ -8444,7 +8441,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="283" spans="1:7">
+    <row r="283" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A283" t="s">
         <v>190</v>
       </c>
@@ -8461,7 +8458,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="285" spans="1:7">
+    <row r="285" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A285" t="s">
         <v>194</v>
       </c>
@@ -8475,7 +8472,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="287" spans="1:7">
+    <row r="287" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A287" t="s">
         <v>198</v>
       </c>
@@ -8495,7 +8492,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="289" spans="1:6">
+    <row r="289" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A289" t="s">
         <v>203</v>
       </c>
@@ -8509,7 +8506,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="291" spans="1:6">
+    <row r="291" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A291" t="s">
         <v>207</v>
       </c>
@@ -8523,7 +8520,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="293" spans="1:6">
+    <row r="293" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A293" t="s">
         <v>211</v>
       </c>
@@ -8540,7 +8537,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="295" spans="1:6">
+    <row r="295" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A295" t="s">
         <v>215</v>
       </c>
@@ -8554,7 +8551,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="297" spans="1:6">
+    <row r="297" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A297" t="s">
         <v>219</v>
       </c>
@@ -8568,7 +8565,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="299" spans="1:6">
+    <row r="299" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A299" t="s">
         <v>223</v>
       </c>
@@ -8585,7 +8582,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="301" spans="1:6">
+    <row r="301" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A301" t="s">
         <v>227</v>
       </c>
@@ -8599,7 +8596,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="303" spans="1:6">
+    <row r="303" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A303" t="s">
         <v>231</v>
       </c>
@@ -8613,7 +8610,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="305" spans="1:6">
+    <row r="305" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A305" t="s">
         <v>109</v>
       </c>
@@ -8630,7 +8627,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="307" spans="1:6">
+    <row r="307" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A307" t="s">
         <v>113</v>
       </c>
@@ -8644,7 +8641,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="309" spans="1:6">
+    <row r="309" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A309" t="s">
         <v>117</v>
       </c>
@@ -8658,7 +8655,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="311" spans="1:6">
+    <row r="311" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A311" t="s">
         <v>121</v>
       </c>
@@ -8672,7 +8669,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="313" spans="1:6">
+    <row r="313" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A313" t="s">
         <v>125</v>
       </c>
@@ -8686,7 +8683,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="315" spans="1:6">
+    <row r="315" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A315" t="s">
         <v>129</v>
       </c>
@@ -8700,7 +8697,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="317" spans="1:6">
+    <row r="317" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A317" t="s">
         <v>133</v>
       </c>
@@ -8717,7 +8714,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="319" spans="1:6">
+    <row r="319" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A319" t="s">
         <v>136</v>
       </c>
@@ -8731,7 +8728,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="321" spans="1:6">
+    <row r="321" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A321" t="s">
         <v>140</v>
       </c>
@@ -8745,7 +8742,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="323" spans="1:6">
+    <row r="323" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A323" t="s">
         <v>144</v>
       </c>
@@ -8762,7 +8759,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="325" spans="1:6">
+    <row r="325" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A325" t="s">
         <v>148</v>
       </c>
@@ -8779,7 +8776,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="327" spans="1:6">
+    <row r="327" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A327" t="s">
         <v>152</v>
       </c>
@@ -8796,7 +8793,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="329" spans="1:6">
+    <row r="329" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A329" t="s">
         <v>156</v>
       </c>
@@ -8813,7 +8810,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="331" spans="1:6">
+    <row r="331" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A331" t="s">
         <v>160</v>
       </c>
@@ -8830,7 +8827,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="333" spans="1:6">
+    <row r="333" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A333" t="s">
         <v>164</v>
       </c>
@@ -8847,7 +8844,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="335" spans="1:6">
+    <row r="335" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A335" t="s">
         <v>168</v>
       </c>
@@ -8861,7 +8858,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="337" spans="1:11">
+    <row r="337" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A337" t="s">
         <v>52</v>
       </c>
@@ -8881,7 +8878,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="339" spans="1:11">
+    <row r="339" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A339" t="s">
         <v>56</v>
       </c>
@@ -8898,7 +8895,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="341" spans="1:11">
+    <row r="341" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A341" t="s">
         <v>60</v>
       </c>
@@ -8912,7 +8909,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="343" spans="1:11">
+    <row r="343" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A343" t="s">
         <v>64</v>
       </c>
@@ -8929,7 +8926,7 @@
         <v>9952395</v>
       </c>
     </row>
-    <row r="345" spans="1:11">
+    <row r="345" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A345" t="s">
         <v>68</v>
       </c>
@@ -8946,7 +8943,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="347" spans="1:11">
+    <row r="347" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A347" t="s">
         <v>72</v>
       </c>
@@ -8960,7 +8957,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="349" spans="1:11">
+    <row r="349" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A349" t="s">
         <v>76</v>
       </c>
@@ -8980,10 +8977,10 @@
         <v>80</v>
       </c>
     </row>
-    <row r="350" spans="1:11">
+    <row r="350" spans="1:11" x14ac:dyDescent="0.15">
       <c r="H350" s="19"/>
     </row>
-    <row r="351" spans="1:11" ht="21">
+    <row r="351" spans="1:11" ht="23" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
         <v>81</v>
       </c>
@@ -8998,10 +8995,10 @@
       </c>
       <c r="H351" s="20"/>
     </row>
-    <row r="352" spans="1:11">
+    <row r="352" spans="1:11" x14ac:dyDescent="0.15">
       <c r="H352" s="19"/>
     </row>
-    <row r="353" spans="1:11">
+    <row r="353" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A353" t="s">
         <v>85</v>
       </c>
@@ -9021,7 +9018,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="355" spans="1:11">
+    <row r="355" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A355" t="s">
         <v>90</v>
       </c>
@@ -9038,7 +9035,7 @@
         <v>24462093</v>
       </c>
     </row>
-    <row r="357" spans="1:11">
+    <row r="357" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A357" t="s">
         <v>94</v>
       </c>
@@ -9055,7 +9052,7 @@
         <v>24462093</v>
       </c>
     </row>
-    <row r="359" spans="1:11">
+    <row r="359" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A359" t="s">
         <v>98</v>
       </c>
@@ -9072,7 +9069,7 @@
         <v>24462093</v>
       </c>
     </row>
-    <row r="361" spans="1:11">
+    <row r="361" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A361" t="s">
         <v>102</v>
       </c>
@@ -9089,7 +9086,7 @@
         <v>24462093</v>
       </c>
     </row>
-    <row r="363" spans="1:11">
+    <row r="363" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A363" t="s">
         <v>105</v>
       </c>
@@ -9112,7 +9109,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="365" spans="1:11">
+    <row r="365" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A365" t="s">
         <v>3</v>
       </c>
@@ -9126,7 +9123,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="367" spans="1:11">
+    <row r="367" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A367" t="s">
         <v>7</v>
       </c>
@@ -9140,7 +9137,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="369" spans="1:11">
+    <row r="369" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A369" t="s">
         <v>11</v>
       </c>
@@ -9154,7 +9151,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="371" spans="1:11">
+    <row r="371" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A371" t="s">
         <v>15</v>
       </c>
@@ -9168,7 +9165,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="373" spans="1:11">
+    <row r="373" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A373" t="s">
         <v>19</v>
       </c>
@@ -9182,7 +9179,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="375" spans="1:11" ht="19">
+    <row r="375" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
         <v>23</v>
       </c>
@@ -9202,7 +9199,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="377" spans="1:11">
+    <row r="377" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A377" t="s">
         <v>28</v>
       </c>
@@ -9216,7 +9213,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="379" spans="1:11">
+    <row r="379" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A379" t="s">
         <v>32</v>
       </c>
@@ -9230,7 +9227,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="381" spans="1:11">
+    <row r="381" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A381" t="s">
         <v>36</v>
       </c>
@@ -9244,7 +9241,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="383" spans="1:11" ht="21">
+    <row r="383" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
         <v>40</v>
       </c>
@@ -9267,12 +9264,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="384" spans="1:11">
+    <row r="384" spans="1:11" x14ac:dyDescent="0.15">
       <c r="J384" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="385" spans="1:11" ht="21">
+    <row r="385" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
         <v>47</v>
       </c>
@@ -9290,17 +9287,11 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="24" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="L59" r:id="rId1" location="bib67"/>
     <hyperlink ref="G287" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>